<commit_message>
Committing code for the user type selection
</commit_message>
<xml_diff>
--- a/Tests/Alkermies_creds.xlsx
+++ b/Tests/Alkermies_creds.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git work\Alkermies-code\Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git work\AlkermiesDBS\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8767CC55-0907-4DC7-AA81-C2B65C7B6A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416A89F8-1CF6-4BA6-9D3A-298EB03CCC5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{279C55CB-6DE2-41A3-9563-3FFAA61EBD5B}"/>
+    <workbookView xWindow="2196" yWindow="2196" windowWidth="10440" windowHeight="8964" xr2:uid="{279C55CB-6DE2-41A3-9563-3FFAA61EBD5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Username</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>Digital@trd</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>Trade</t>
   </si>
 </sst>
 </file>
@@ -127,10 +133,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -446,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94368A48-A63F-40F3-AC76-FF849595E27C}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,23 +465,29 @@
     <col min="2" max="2" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -482,7 +495,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -491,6 +504,11 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{8A29336B-CE66-46E7-9695-F65F06F5411B}">
+      <formula1>"Kam, Mmd, Trade"</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{4E97F5C9-496B-4382-ACA5-26F9982AB400}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{D64671A6-9B48-4F45-A867-7E672F78A661}"/>

</xml_diff>